<commit_message>
feat: Case two completed
</commit_message>
<xml_diff>
--- a/Roberto.xlsx
+++ b/Roberto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,55 +436,31 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Dueño</t>
+          <t>Puntuación promedio de los airbnb de la zona de Roberto y Clara</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>ID habitación</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Cantidad reseñas</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Puntuación (0 a 5)</t>
-        </is>
+      <c r="B1" t="n">
+        <v>3.3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Clara</t>
+          <t>Reseñas promedio de los airbnb de la zona de Roberto y Clara</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90387</v>
-      </c>
-      <c r="C2" t="n">
-        <v>204</v>
-      </c>
-      <c r="D2" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Roberto</t>
+          <t>Precio promedio de los airbnb de la zona de Roberto y Clara</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>97503</v>
-      </c>
-      <c r="C3" t="n">
-        <v>39</v>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
+        <v>83.59999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Last changes added to handle errors and other
</commit_message>
<xml_diff>
--- a/Roberto.xlsx
+++ b/Roberto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,66 @@
         <v>83.59999999999999</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Puntuación general airbnb de Clara: </t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cantidad reseñas airbnb de Clara: </t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Precio por noche airbnb de Clara: </t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Puntuación general airbnb de Roberto: </t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cantidad reseñas airbnb de Roberto: </t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Precio por noche airbnb de Roberto: </t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>